<commit_message>
Added excel view feature
</commit_message>
<xml_diff>
--- a/backend/uploads/Adsız 1.xlsx
+++ b/backend/uploads/Adsız 1.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,6 +27,12 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -55,11 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -456,7 +463,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="2" t="n">
         <v>45370086520</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -474,7 +481,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="2" t="n">
         <v>35815359920</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -492,7 +499,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="2" t="n">
         <v>14887218076</v>
       </c>
       <c r="B4" t="inlineStr">

</xml_diff>